<commit_message>
began adc testing for current sensor
Ran into issues with power mosfets on board. Will revisit tomorrow.
</commit_message>
<xml_diff>
--- a/adc_code.xlsx
+++ b/adc_code.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxwe\Documents\GitHub\Bms_Software\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxwe\Documents\Energia\libraries\Bms_Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EC05B01-459E-4A12-89F4-032E949CD6A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15144A6-4090-4821-8DA3-B30B8CB93DD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2166" yWindow="2166" windowWidth="17280" windowHeight="10524" xr2:uid="{E4629A19-C78F-4488-ABB5-0BC9F7658780}"/>
+    <workbookView xWindow="3300" yWindow="3474" windowWidth="3456" windowHeight="1824" activeTab="1" xr2:uid="{E4629A19-C78F-4488-ABB5-0BC9F7658780}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="cellVoltage" sheetId="1" r:id="rId1"/>
+    <sheet name="currentADC" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="14">
   <si>
     <t>Cell1</t>
   </si>
@@ -70,6 +71,12 @@
   </si>
   <si>
     <t>VOLTAGE @ TIVA</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>ADC Value</t>
   </si>
 </sst>
 </file>
@@ -438,7 +445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB12396-80DD-4524-8C53-E9156979B265}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -1417,4 +1424,32 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{154FB61A-6E3B-40BD-9756-95AE3477DBE3}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>